<commit_message>
added option to exclude retweets
</commit_message>
<xml_diff>
--- a/docs/graphs/tone_frequencies+retweets.xlsx
+++ b/docs/graphs/tone_frequencies+retweets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olddominion-my.sharepoint.com/personal/jmart130_odu_edu/Documents/GitHub/twitter_analysis_col/docs/graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="512" documentId="11_4C1CE49650B0F515CA3E72BFC370B3F462223BE8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3FDE682-5789-42BE-9922-797625725A9F}"/>
+  <xr:revisionPtr revIDLastSave="530" documentId="11_4C1CE49650B0F515CA3E72BFC370B3F462223BE8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{797ADB65-6783-4031-B5D4-01F5AFFB006B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{61C9C911-FF89-4C19-BE5A-DC4DFBA47279}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{61C9C911-FF89-4C19-BE5A-DC4DFBA47279}"/>
   </bookViews>
   <sheets>
     <sheet name="yearly" sheetId="11" r:id="rId1"/>
@@ -451,6 +451,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -579,8 +580,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBA6212"/>
+      <color rgb="FFEE9949"/>
+      <color rgb="FF828282"/>
       <color rgb="FFC6C6C6"/>
-      <color rgb="FFEE9949"/>
+      <color rgb="FF2F76A1"/>
       <color rgb="FF4899C9"/>
     </mruColors>
   </colors>
@@ -5763,6 +5767,2611 @@
         <c:crossAx val="1374323584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tone frequency without</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> retweets </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>- monthly</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'monthly - no RT'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>negative</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="EE9949"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="70"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.5026901830507901E-2"/>
+                  <c:y val="-4.9257883076281088E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-E34C-4A6D-A81D-BC631E46B029}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="81"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5821192640774973E-2"/>
+                  <c:y val="-8.6060824395402802E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="4.8303853322682479E-2"/>
+                      <c:h val="6.7523992170229474E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E34C-4A6D-A81D-BC631E46B029}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="86"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2938871771463348E-2"/>
+                  <c:y val="-6.0879912709711291E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-E34C-4A6D-A81D-BC631E46B029}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="EE9949"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.2966935896297988E-2"/>
+                  <c:y val="-8.4258189641629677E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="BA6212"/>
+                      </a:solidFill>
+                      <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'monthly - no RT'!$E$2:$E$103</c:f>
+              <c:strCache>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>2014-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2014-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2014-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2014-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2014-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2014-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2014-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2014-12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2015-01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2015-02</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2015-03</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015-04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2015-05</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2015-06</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2015-07</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015-08</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015-09</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2015-10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2015-11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2015-12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2016-01</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2016-02</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2016-03</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2016-04</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2016-05</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2016-06</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2016-07</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2016-08</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2016-09</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2016-10</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2016-11</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2016-12</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2017-01</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2017-02</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2017-03</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2017-04</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2017-05</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2017-06</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2017-07</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2017-08</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2017-09</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2017-10</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2017-11</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2017-12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2018-01</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2018-02</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2018-03</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2018-04</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2018-05</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2018-06</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2018-07</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2018-08</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2018-09</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2018-10</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2018-11</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2018-12</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2019-01</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2019-02</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2019-03</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2019-04</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2019-05</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2019-06</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2019-07</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2019-08</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2019-09</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2019-10</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2019-11</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2019-12</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2021-01</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2021-02</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2021-03</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2021-04</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2021-05</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2021-06</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2021-07</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2021-08</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2021-09</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2021-10</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2021-11</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2021-12</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2022-01</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2022-02</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2022-03</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2022-04</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2022-05</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2022-06</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'monthly - no RT'!$I$2:$I$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>682</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1790</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2292</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1458</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2421</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1284</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>854</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1939</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1724</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3106</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2813</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2133</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2223</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1752</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3869</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3426</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3254</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3389</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2763</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4350</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4775</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3850</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2996</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3805</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4385</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3475</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4402</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4676</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4008</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>12982</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3997</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5007</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5081</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9200</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9833</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6031</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8802</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6881</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6357</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>7080</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>12219</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8861</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6900</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>7310</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9017</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>12673</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7249</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8604</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7583</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6382</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9729</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6097</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6615</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5240</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5890</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>7088</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>8547</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>7215</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>7607</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>7508</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>8698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E34C-4A6D-A81D-BC631E46B029}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'monthly - no RT'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neutral</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C6C6C6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C6C6C6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.8517081500078192E-2"/>
+                  <c:y val="-3.2410515710025178E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="828282"/>
+                      </a:solidFill>
+                      <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'monthly - no RT'!$E$2:$E$103</c:f>
+              <c:strCache>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>2014-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2014-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2014-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2014-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2014-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2014-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2014-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2014-12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2015-01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2015-02</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2015-03</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015-04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2015-05</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2015-06</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2015-07</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015-08</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015-09</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2015-10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2015-11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2015-12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2016-01</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2016-02</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2016-03</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2016-04</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2016-05</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2016-06</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2016-07</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2016-08</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2016-09</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2016-10</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2016-11</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2016-12</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2017-01</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2017-02</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2017-03</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2017-04</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2017-05</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2017-06</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2017-07</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2017-08</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2017-09</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2017-10</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2017-11</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2017-12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2018-01</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2018-02</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2018-03</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2018-04</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2018-05</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2018-06</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2018-07</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2018-08</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2018-09</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2018-10</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2018-11</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2018-12</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2019-01</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2019-02</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2019-03</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2019-04</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2019-05</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2019-06</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2019-07</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2019-08</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2019-09</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2019-10</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2019-11</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2019-12</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2021-01</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2021-02</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2021-03</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2021-04</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2021-05</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2021-06</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2021-07</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2021-08</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2021-09</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2021-10</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2021-11</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2021-12</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2022-01</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2022-02</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2022-03</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2022-04</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2022-05</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2022-06</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'monthly - no RT'!$J$2:$J$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>591</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>762</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>891</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1261</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1954</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1365</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1245</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1089</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2145</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1924</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2365</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1774</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1553</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2461</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1922</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1762</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2419</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1765</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2444</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2080</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1811</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3212</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1908</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2224</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2437</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4086</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3147</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6335</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3513</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3436</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3263</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5136</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4087</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3338</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3282</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4765</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4915</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3291</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3455</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4118</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3848</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3961</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2990</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3726</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2995</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3069</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2924</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3702</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3224</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3530</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3770</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3671</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E34C-4A6D-A81D-BC631E46B029}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'monthly - no RT'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>positive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="4899C9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="4899C9"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.0819861285455259E-2"/>
+                  <c:y val="6.0430283531767034E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="2F76A1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'monthly - no RT'!$E$2:$E$103</c:f>
+              <c:strCache>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>2014-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014-02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014-03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2014-04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014-05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2014-06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2014-07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2014-08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2014-09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2014-10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014-11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2014-12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2015-01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2015-02</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2015-03</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015-04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2015-05</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2015-06</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2015-07</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015-08</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015-09</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2015-10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2015-11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2015-12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2016-01</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2016-02</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2016-03</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2016-04</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2016-05</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2016-06</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2016-07</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2016-08</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2016-09</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2016-10</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2016-11</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2016-12</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2017-01</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2017-02</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2017-03</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2017-04</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2017-05</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2017-06</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2017-07</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2017-08</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2017-09</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2017-10</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2017-11</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2017-12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2018-01</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2018-02</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2018-03</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2018-04</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2018-05</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2018-06</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2018-07</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2018-08</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2018-09</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2018-10</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2018-11</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2018-12</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2019-01</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2019-02</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2019-03</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2019-04</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2019-05</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2019-06</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2019-07</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2019-08</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2019-09</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2019-10</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2019-11</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2019-12</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2020-01</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2020-02</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2020-03</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2020-04</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2020-05</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2020-06</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2020-07</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2020-08</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2020-09</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2020-10</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2020-11</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2020-12</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2021-01</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2021-02</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2021-03</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2021-04</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2021-05</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2021-06</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2021-07</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2021-08</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2021-09</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2021-10</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2021-11</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2021-12</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2022-01</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2022-02</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2022-03</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2022-04</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2022-05</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2022-06</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'monthly - no RT'!$K$2:$K$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>613</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>669</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>691</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>408</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>975</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>866</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>765</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1785</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1407</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1585</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1417</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1469</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1959</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1567</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1268</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1689</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1919</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1467</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1688</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1576</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1451</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2768</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1503</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1571</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1519</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3563</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2258</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3860</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2587</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2468</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2534</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3833</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3114</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2998</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2461</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4186</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3821</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2644</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2620</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3274</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2952</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3522</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2293</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2474</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2364</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2474</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2130</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2844</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2508</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2626</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E34C-4A6D-A81D-BC631E46B029}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1374323584"/>
+        <c:axId val="1374307776"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1374323584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1374307776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="12"/>
+        <c:tickMarkSkip val="12"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1374307776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1374323584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -21647,6 +24256,43 @@
 </file>
 
 <file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
@@ -25851,6 +28497,527 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -26287,6 +29454,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>399731</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>139148</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6D0AEEF-130B-42B0-AF6C-100B45679117}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -29389,8 +32594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AG54" sqref="AG54"/>
+    <sheetView topLeftCell="M38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z66" sqref="Z66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36900,8 +40105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K511"/>
   <sheetViews>
-    <sheetView topLeftCell="N35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Z67" sqref="Z67"/>
+    <sheetView tabSelected="1" topLeftCell="P56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AH74" sqref="AH74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>